<commit_message>
Implemented Diagnostic mode & System class
Diagnostic Mode:
- Enter diagnostic mode after soft-reset

System
- now dedicated class
</commit_message>
<xml_diff>
--- a/Datasheets/DataFormat.xlsx
+++ b/Datasheets/DataFormat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Desktop\eWheel\Datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FCBCC0-5D05-4C8D-A8D3-C7EDEBCB6369}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED208C48-BE9E-4B30-82E5-9BE725DEA1C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28065" windowHeight="16440" activeTab="1" xr2:uid="{E22249E2-E3E8-45A5-9C21-2EC87B3551B2}"/>
   </bookViews>
@@ -179,9 +179,6 @@
     <t xml:space="preserve">Payload length </t>
   </si>
   <si>
-    <t>Set TraceMode</t>
-  </si>
-  <si>
     <t>0xDEADBEEF</t>
   </si>
   <si>
@@ -195,6 +192,9 @@
   </si>
   <si>
     <t>Mode</t>
+  </si>
+  <si>
+    <t>Set Diagnostic Mode</t>
   </si>
 </sst>
 </file>
@@ -540,12 +540,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -573,6 +597,30 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -592,12 +640,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -606,9 +648,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -617,45 +656,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1006,12 +1006,12 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1149,12 +1149,12 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1200,7 +1200,7 @@
   <dimension ref="A2:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,37 +1224,37 @@
       <c r="E2" s="1">
         <v>4</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="24"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="32"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="26"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="29"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="37"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
@@ -1262,39 +1262,39 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="51" t="s">
+      <c r="C6" s="28"/>
+      <c r="D6" s="19" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="20"/>
+      <c r="B7" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="24"/>
       <c r="D7" s="18">
         <v>1</v>
       </c>
-      <c r="E7" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
+      <c r="E7" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
@@ -1302,63 +1302,58 @@
       <c r="M7" s="17"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="53">
+      <c r="C8" s="27"/>
+      <c r="D8" s="20">
         <v>2</v>
       </c>
-      <c r="E8" s="52" t="s">
+      <c r="E8" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="52"/>
+      <c r="F8" s="27"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="22">
+        <v>3</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="57">
-        <v>3</v>
-      </c>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="18">
         <v>4</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="20"/>
+      <c r="B11" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="24"/>
       <c r="D11" s="18">
         <v>255</v>
       </c>
-      <c r="E11" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
+      <c r="E11" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E4:M4"/>
@@ -1367,6 +1362,11 @@
     <mergeCell ref="E3:M3"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E7:H7"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1429,13 +1429,13 @@
       <c r="N2" s="1">
         <v>12</v>
       </c>
-      <c r="O2" s="22"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="24"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="32"/>
       <c r="V2" s="1">
         <f>N2+64</f>
         <v>76</v>
@@ -1448,37 +1448,37 @@
       <c r="C3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="25" t="s">
+      <c r="E3" s="46"/>
+      <c r="F3" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="26"/>
+      <c r="G3" s="34"/>
       <c r="H3" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="27" t="s">
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="29"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="36"/>
+      <c r="S3" s="36"/>
+      <c r="T3" s="36"/>
+      <c r="U3" s="36"/>
+      <c r="V3" s="37"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
@@ -1493,17 +1493,17 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="21"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="29"/>
+      <c r="V4" s="29"/>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
@@ -1518,17 +1518,17 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="49" t="s">
+      <c r="N5" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -1543,17 +1543,17 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="21" t="s">
+      <c r="N6" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-      <c r="T6" s="21"/>
-      <c r="U6" s="21"/>
-      <c r="V6" s="21"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="29"/>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
@@ -1568,17 +1568,17 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
-      <c r="N7" s="21" t="s">
+      <c r="N7" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
@@ -1593,17 +1593,17 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="21" t="s">
+      <c r="N8" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21"/>
-      <c r="U8" s="21"/>
-      <c r="V8" s="21"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="29"/>
+      <c r="V8" s="29"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
@@ -1618,24 +1618,24 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="21" t="s">
+      <c r="N9" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="29"/>
+      <c r="V9" s="29"/>
     </row>
     <row r="15" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F15" s="47" t="s">
+      <c r="F15" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
       <c r="I15" s="11" t="s">
         <v>28</v>
       </c>
@@ -1671,11 +1671,11 @@
       </c>
     </row>
     <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F16" s="41" t="s">
+      <c r="F16" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
       <c r="I16" s="13">
         <v>1</v>
       </c>
@@ -1691,42 +1691,42 @@
       <c r="S16" s="14"/>
     </row>
     <row r="17" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="F17" s="39" t="s">
+      <c r="F17" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
       <c r="I17" s="10">
         <v>2</v>
       </c>
-      <c r="J17" s="37" t="s">
+      <c r="J17" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="38"/>
-      <c r="L17" s="45" t="s">
+      <c r="K17" s="41"/>
+      <c r="L17" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="M17" s="46"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="46"/>
-      <c r="P17" s="46"/>
-      <c r="Q17" s="46"/>
-      <c r="R17" s="46"/>
-      <c r="S17" s="46"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="39"/>
+      <c r="S17" s="39"/>
     </row>
     <row r="18" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
       <c r="I18" s="6">
         <v>3</v>
       </c>
-      <c r="J18" s="37" t="s">
+      <c r="J18" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="38"/>
+      <c r="K18" s="41"/>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
       <c r="N18" s="16"/>
@@ -1737,57 +1737,57 @@
       <c r="S18" s="16"/>
     </row>
     <row r="19" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="42" t="s">
+      <c r="F19" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="43"/>
-      <c r="H19" s="44"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="57"/>
       <c r="I19" s="13">
         <v>4</v>
       </c>
-      <c r="J19" s="34" t="s">
+      <c r="J19" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="35"/>
-      <c r="S19" s="35"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="51"/>
+      <c r="Q19" s="51"/>
+      <c r="R19" s="51"/>
+      <c r="S19" s="51"/>
     </row>
     <row r="20" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="F20" s="39" t="s">
+      <c r="F20" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
       <c r="I20" s="10">
         <v>63</v>
       </c>
-      <c r="J20" s="31" t="s">
+      <c r="J20" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="31" t="s">
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="33"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="49"/>
       <c r="R20" s="16"/>
       <c r="S20" s="16"/>
     </row>
     <row r="21" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="F21" s="40" t="s">
+      <c r="F21" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
       <c r="I21" s="7">
         <v>64</v>
       </c>
@@ -1803,26 +1803,26 @@
       <c r="S21" s="16"/>
     </row>
     <row r="22" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="41" t="s">
+      <c r="F22" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
       <c r="I22" s="13">
         <v>65</v>
       </c>
-      <c r="J22" s="34" t="s">
+      <c r="J22" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="34" t="s">
+      <c r="K22" s="51"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="O22" s="35"/>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="36"/>
+      <c r="O22" s="51"/>
+      <c r="P22" s="51"/>
+      <c r="Q22" s="52"/>
       <c r="R22" s="14"/>
       <c r="S22" s="14"/>
     </row>
@@ -1831,19 +1831,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="O2:U2"/>
-    <mergeCell ref="L17:S17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="N4:V4"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:V3"/>
-    <mergeCell ref="N5:V5"/>
-    <mergeCell ref="N6:V6"/>
-    <mergeCell ref="N7:V7"/>
-    <mergeCell ref="N8:V8"/>
-    <mergeCell ref="N9:V9"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J20:M20"/>
@@ -1858,6 +1845,19 @@
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="F19:H19"/>
+    <mergeCell ref="O2:U2"/>
+    <mergeCell ref="L17:S17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="N4:V4"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:V3"/>
+    <mergeCell ref="N5:V5"/>
+    <mergeCell ref="N6:V6"/>
+    <mergeCell ref="N7:V7"/>
+    <mergeCell ref="N8:V8"/>
+    <mergeCell ref="N9:V9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implemented cyclic readout of analog values for IR-sensor front and back
</commit_message>
<xml_diff>
--- a/Datasheets/DataFormat.xlsx
+++ b/Datasheets/DataFormat.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Desktop\eWheel\Datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED208C48-BE9E-4B30-82E5-9BE725DEA1C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A19149-1CF6-4E51-ADC7-99ADFEA94454}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28065" windowHeight="16440" activeTab="1" xr2:uid="{E22249E2-E3E8-45A5-9C21-2EC87B3551B2}"/>
+    <workbookView xWindow="7005" yWindow="600" windowWidth="20865" windowHeight="11835" activeTab="2" xr2:uid="{E22249E2-E3E8-45A5-9C21-2EC87B3551B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="CP2102 DataPacket" sheetId="3" r:id="rId2"/>
-    <sheet name="CC41A DataPacket" sheetId="2" r:id="rId3"/>
+    <sheet name="IR" sheetId="4" r:id="rId3"/>
+    <sheet name="CC41A DataPacket" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>Value</t>
   </si>
@@ -195,6 +196,18 @@
   </si>
   <si>
     <t>Set Diagnostic Mode</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -512,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -555,6 +568,39 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -564,38 +610,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -603,60 +661,16 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -672,6 +686,1253 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IR!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>IR!$A$2:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>IR!$B$2:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.92</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.4800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.76</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.36</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.68</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.96</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.44</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.84</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.28</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.32</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.9600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.68</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10.64</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12.88</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14.36</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16.28</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18.88</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22.16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26.16</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>32.72</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40.28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BF6C-4112-8843-6A46B342F449}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IR!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>IR!$A$2:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>IR!$C$2:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>3.548921834194934</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.70157996594771</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8665154191003568</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0452089974929528</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2393842164859761</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.4510584360155736</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.682607357575721</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.9368471143110719</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.2171397761153218</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5275303890992085</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.8729270339689208</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.2593403997065415</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.6942069702755083</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.1868316832400545</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.7490045215398959</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.3958756488752844</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.147223909086069</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10.029339718465538</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11.077896590425372</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12.3424687410738</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13.8939</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15.836846207410774</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18.33223762173391</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>21.640080582537596</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26.207576996524558</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>32.869548028343772</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43.369562540006292</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001B-BF6C-4112-8843-6A46B342F449}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="24346367"/>
+        <c:axId val="1986161023"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="24346367"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1986161023"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1986161023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="24346367"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>633411</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96EEC762-ED77-4EE5-BE0F-8EF97733A6E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1199,7 +2460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1AC88FD-8444-4667-A8F6-2D07972D95E5}">
   <dimension ref="A2:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -1224,37 +2485,37 @@
       <c r="E2" s="1">
         <v>4</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="32"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="29"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="37"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="34"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
@@ -1262,39 +2523,39 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="19" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="24"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="18">
         <v>1</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
@@ -1302,23 +2563,23 @@
       <c r="M7" s="17"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="27"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="20">
         <v>2</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="25"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="26"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="22">
         <v>3</v>
       </c>
@@ -1326,10 +2587,10 @@
       <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="24"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="18">
         <v>4</v>
       </c>
@@ -1338,22 +2599,27 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="24"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="18">
         <v>255</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E4:M4"/>
@@ -1362,17 +2628,376 @@
     <mergeCell ref="E3:M3"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E7:H7"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB83D9D3-B3A2-4544-B5AF-185922725977}">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="58"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="58">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3.4</v>
+      </c>
+      <c r="C2">
+        <f>13.8939*A2^-1.2423</f>
+        <v>3.548921834194934</v>
+      </c>
+      <c r="E2">
+        <v>13.8939</v>
+      </c>
+      <c r="F2">
+        <v>-1.2423</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="58">
+        <v>2.9</v>
+      </c>
+      <c r="B3">
+        <v>3.52</v>
+      </c>
+      <c r="C3">
+        <f>13.8939*A3^-1.2423</f>
+        <v>3.70157996594771</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="58">
+        <v>2.8</v>
+      </c>
+      <c r="B4">
+        <v>3.76</v>
+      </c>
+      <c r="C4">
+        <f>13.8939*A4^-1.2423</f>
+        <v>3.8665154191003568</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="58">
+        <v>2.7</v>
+      </c>
+      <c r="B5">
+        <v>3.92</v>
+      </c>
+      <c r="C5">
+        <f>13.8939*A5^-1.2423</f>
+        <v>4.0452089974929528</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="58">
+        <v>2.6</v>
+      </c>
+      <c r="B6">
+        <v>4.24</v>
+      </c>
+      <c r="C6">
+        <f>13.8939*A6^-1.2423</f>
+        <v>4.2393842164859761</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="58">
+        <v>2.5</v>
+      </c>
+      <c r="B7">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="C7">
+        <f>13.8939*A7^-1.2423</f>
+        <v>4.4510584360155736</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="58">
+        <v>2.4</v>
+      </c>
+      <c r="B8">
+        <v>4.76</v>
+      </c>
+      <c r="C8">
+        <f>13.8939*A8^-1.2423</f>
+        <v>4.682607357575721</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="58">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B9">
+        <v>5.04</v>
+      </c>
+      <c r="C9">
+        <f>13.8939*A9^-1.2423</f>
+        <v>4.9368471143110719</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="58">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B10">
+        <v>5.36</v>
+      </c>
+      <c r="C10">
+        <f>13.8939*A10^-1.2423</f>
+        <v>5.2171397761153218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="58">
+        <v>2.1</v>
+      </c>
+      <c r="B11">
+        <v>5.68</v>
+      </c>
+      <c r="C11">
+        <f>13.8939*A11^-1.2423</f>
+        <v>5.5275303890992085</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="58">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>5.96</v>
+      </c>
+      <c r="C12">
+        <f>13.8939*A12^-1.2423</f>
+        <v>5.8729270339689208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="58">
+        <v>1.9</v>
+      </c>
+      <c r="B13">
+        <v>6.44</v>
+      </c>
+      <c r="C13">
+        <f>13.8939*A13^-1.2423</f>
+        <v>6.2593403997065415</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="58">
+        <v>1.8</v>
+      </c>
+      <c r="B14">
+        <v>6.84</v>
+      </c>
+      <c r="C14">
+        <f>13.8939*A14^-1.2423</f>
+        <v>6.6942069702755083</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="58">
+        <v>1.7</v>
+      </c>
+      <c r="B15">
+        <v>7.28</v>
+      </c>
+      <c r="C15">
+        <f>13.8939*A15^-1.2423</f>
+        <v>7.1868316832400545</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="58">
+        <v>1.6</v>
+      </c>
+      <c r="B16">
+        <v>7.8</v>
+      </c>
+      <c r="C16">
+        <f>13.8939*A16^-1.2423</f>
+        <v>7.7490045215398959</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="58">
+        <v>1.5</v>
+      </c>
+      <c r="B17">
+        <v>8.32</v>
+      </c>
+      <c r="C17">
+        <f>13.8939*A17^-1.2423</f>
+        <v>8.3958756488752844</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="58">
+        <v>1.4</v>
+      </c>
+      <c r="B18">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="C18">
+        <f>13.8939*A18^-1.2423</f>
+        <v>9.147223909086069</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="58">
+        <v>1.3</v>
+      </c>
+      <c r="B19">
+        <v>9.68</v>
+      </c>
+      <c r="C19">
+        <f>13.8939*A19^-1.2423</f>
+        <v>10.029339718465538</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="58">
+        <v>1.2</v>
+      </c>
+      <c r="B20">
+        <v>10.64</v>
+      </c>
+      <c r="C20">
+        <f>13.8939*A20^-1.2423</f>
+        <v>11.077896590425372</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="58">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B21">
+        <v>12.88</v>
+      </c>
+      <c r="C21">
+        <f>13.8939*A21^-1.2423</f>
+        <v>12.3424687410738</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="58">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>14.36</v>
+      </c>
+      <c r="C22">
+        <f>13.8939*A22^-1.2423</f>
+        <v>13.8939</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="B23">
+        <v>16.28</v>
+      </c>
+      <c r="C23">
+        <f>13.8939*A23^-1.2423</f>
+        <v>15.836846207410774</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="58">
+        <v>0.8</v>
+      </c>
+      <c r="B24">
+        <v>18.88</v>
+      </c>
+      <c r="C24">
+        <f>13.8939*A24^-1.2423</f>
+        <v>18.33223762173391</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="58">
+        <v>0.7</v>
+      </c>
+      <c r="B25">
+        <v>22.16</v>
+      </c>
+      <c r="C25">
+        <f>13.8939*A25^-1.2423</f>
+        <v>21.640080582537596</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="58">
+        <v>0.6</v>
+      </c>
+      <c r="B26">
+        <v>26.16</v>
+      </c>
+      <c r="C26">
+        <f>13.8939*A26^-1.2423</f>
+        <v>26.207576996524558</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="B27">
+        <v>32.72</v>
+      </c>
+      <c r="C27">
+        <f>13.8939*A27^-1.2423</f>
+        <v>32.869548028343772</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="58">
+        <v>0.4</v>
+      </c>
+      <c r="B28">
+        <v>40.28</v>
+      </c>
+      <c r="C28">
+        <f>13.8939*A28^-1.2423</f>
+        <v>43.369562540006292</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD17DA2-D66C-4765-8B42-9B8593C77046}">
   <dimension ref="B2:V23"/>
   <sheetViews>
@@ -1429,13 +3054,13 @@
       <c r="N2" s="1">
         <v>12</v>
       </c>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="32"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="29"/>
       <c r="V2" s="1">
         <f>N2+64</f>
         <v>76</v>
@@ -1448,37 +3073,37 @@
       <c r="C3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="33" t="s">
+      <c r="E3" s="38"/>
+      <c r="F3" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="34"/>
+      <c r="G3" s="31"/>
       <c r="H3" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="35" t="s">
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36"/>
-      <c r="U3" s="36"/>
-      <c r="V3" s="37"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="33"/>
+      <c r="V3" s="34"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
@@ -1493,17 +3118,17 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="29" t="s">
+      <c r="N4" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="29"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
+      <c r="V4" s="26"/>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
@@ -1518,17 +3143,17 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="45" t="s">
+      <c r="N5" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -1543,17 +3168,17 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="29" t="s">
+      <c r="N6" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="29"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="29"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
@@ -1568,17 +3193,17 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
-      <c r="N7" s="29" t="s">
+      <c r="N7" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="29"/>
-      <c r="T7" s="29"/>
-      <c r="U7" s="29"/>
-      <c r="V7" s="29"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="26"/>
+      <c r="V7" s="26"/>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
@@ -1593,17 +3218,17 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="29" t="s">
+      <c r="N8" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
-      <c r="S8" s="29"/>
-      <c r="T8" s="29"/>
-      <c r="U8" s="29"/>
-      <c r="V8" s="29"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="26"/>
+      <c r="S8" s="26"/>
+      <c r="T8" s="26"/>
+      <c r="U8" s="26"/>
+      <c r="V8" s="26"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
@@ -1618,24 +3243,24 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="29" t="s">
+      <c r="N9" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="29"/>
-      <c r="V9" s="29"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="26"/>
+      <c r="T9" s="26"/>
+      <c r="U9" s="26"/>
+      <c r="V9" s="26"/>
     </row>
     <row r="15" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
       <c r="I15" s="11" t="s">
         <v>28</v>
       </c>
@@ -1671,11 +3296,11 @@
       </c>
     </row>
     <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F16" s="43" t="s">
+      <c r="F16" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
       <c r="I16" s="13">
         <v>1</v>
       </c>
@@ -1691,42 +3316,42 @@
       <c r="S16" s="14"/>
     </row>
     <row r="17" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="F17" s="53" t="s">
+      <c r="F17" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
       <c r="I17" s="10">
         <v>2</v>
       </c>
-      <c r="J17" s="40" t="s">
+      <c r="J17" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="41"/>
-      <c r="L17" s="38" t="s">
+      <c r="K17" s="46"/>
+      <c r="L17" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="39"/>
-      <c r="R17" s="39"/>
-      <c r="S17" s="39"/>
+      <c r="M17" s="54"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="54"/>
+      <c r="P17" s="54"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="54"/>
+      <c r="S17" s="54"/>
     </row>
     <row r="18" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
       <c r="I18" s="6">
         <v>3</v>
       </c>
-      <c r="J18" s="40" t="s">
+      <c r="J18" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="41"/>
+      <c r="K18" s="46"/>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
       <c r="N18" s="16"/>
@@ -1737,57 +3362,57 @@
       <c r="S18" s="16"/>
     </row>
     <row r="19" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="55" t="s">
+      <c r="F19" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="56"/>
-      <c r="H19" s="57"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="52"/>
       <c r="I19" s="13">
         <v>4</v>
       </c>
-      <c r="J19" s="50" t="s">
+      <c r="J19" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="51"/>
-      <c r="P19" s="51"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="51"/>
-      <c r="S19" s="51"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="43"/>
+      <c r="R19" s="43"/>
+      <c r="S19" s="43"/>
     </row>
     <row r="20" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
       <c r="I20" s="10">
         <v>63</v>
       </c>
-      <c r="J20" s="47" t="s">
+      <c r="J20" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="47" t="s">
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="O20" s="48"/>
-      <c r="P20" s="48"/>
-      <c r="Q20" s="49"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="41"/>
       <c r="R20" s="16"/>
       <c r="S20" s="16"/>
     </row>
     <row r="21" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="F21" s="54" t="s">
+      <c r="F21" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
       <c r="I21" s="7">
         <v>64</v>
       </c>
@@ -1803,26 +3428,26 @@
       <c r="S21" s="16"/>
     </row>
     <row r="22" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="43" t="s">
+      <c r="F22" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
       <c r="I22" s="13">
         <v>65</v>
       </c>
-      <c r="J22" s="50" t="s">
+      <c r="J22" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="K22" s="51"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="50" t="s">
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="O22" s="51"/>
-      <c r="P22" s="51"/>
-      <c r="Q22" s="52"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="44"/>
       <c r="R22" s="14"/>
       <c r="S22" s="14"/>
     </row>
@@ -1831,6 +3456,19 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="O2:U2"/>
+    <mergeCell ref="L17:S17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="N4:V4"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:V3"/>
+    <mergeCell ref="N5:V5"/>
+    <mergeCell ref="N6:V6"/>
+    <mergeCell ref="N7:V7"/>
+    <mergeCell ref="N8:V8"/>
+    <mergeCell ref="N9:V9"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J20:M20"/>
@@ -1845,19 +3483,6 @@
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="F19:H19"/>
-    <mergeCell ref="O2:U2"/>
-    <mergeCell ref="L17:S17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="N4:V4"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:V3"/>
-    <mergeCell ref="N5:V5"/>
-    <mergeCell ref="N6:V6"/>
-    <mergeCell ref="N7:V7"/>
-    <mergeCell ref="N8:V8"/>
-    <mergeCell ref="N9:V9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implemented BLE basic communication
</commit_message>
<xml_diff>
--- a/Datasheets/DataFormat.xlsx
+++ b/Datasheets/DataFormat.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Desktop\eWheel\Datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9E84A6-1480-4F51-B127-A0D9AD75D68E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225CEF6B-7DD4-44A1-BCA4-E8964A26DB51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28065" windowHeight="16440" activeTab="1" xr2:uid="{E22249E2-E3E8-45A5-9C21-2EC87B3551B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28065" windowHeight="16440" activeTab="2" xr2:uid="{E22249E2-E3E8-45A5-9C21-2EC87B3551B2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="CP2102 DataPacket" sheetId="3" r:id="rId2"/>
-    <sheet name="GP2Y" sheetId="4" r:id="rId3"/>
-    <sheet name="CC41A DataPacket" sheetId="2" r:id="rId4"/>
+    <sheet name="CP2102 DataPacket" sheetId="3" r:id="rId1"/>
+    <sheet name="GP2Y" sheetId="4" r:id="rId2"/>
+    <sheet name="CC41A DataPacket" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,123 +33,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>TempFET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CurrentMotor </t>
-  </si>
-  <si>
-    <t>CurrentIn</t>
-  </si>
-  <si>
-    <t>Duty</t>
-  </si>
-  <si>
-    <t>RPM</t>
-  </si>
-  <si>
-    <t>Vin</t>
-  </si>
-  <si>
-    <t>Ah</t>
-  </si>
-  <si>
-    <t>Wh</t>
-  </si>
-  <si>
-    <t>FaultCode</t>
-  </si>
-  <si>
-    <t>Size [Bytes]</t>
-  </si>
-  <si>
-    <t>cycletime [ms]</t>
-  </si>
-  <si>
-    <t>Bytes/s</t>
-  </si>
-  <si>
-    <t>VESC</t>
-  </si>
-  <si>
-    <t>LSM9D</t>
-  </si>
-  <si>
-    <t>Pitch</t>
-  </si>
-  <si>
-    <t>Roll</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>Payload</t>
-  </si>
-  <si>
-    <t>Seq</t>
   </si>
   <si>
     <t>Length</t>
   </si>
   <si>
-    <t>Flag</t>
-  </si>
-  <si>
-    <t>SrcSwc</t>
-  </si>
-  <si>
-    <t>DstSwc</t>
-  </si>
-  <si>
-    <t>Payload length (bytes)</t>
-  </si>
-  <si>
-    <t>position of payload within complete data set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">receiving component </t>
-  </si>
-  <si>
-    <t>sending component</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0 | 0 | 0 | 0 | 0 | 0 | FIN | ACK</t>
-  </si>
-  <si>
     <t>CMD</t>
-  </si>
-  <si>
-    <t>Page Index</t>
-  </si>
-  <si>
-    <t>Acknoledge Command</t>
-  </si>
-  <si>
-    <t>Set Drive Config</t>
-  </si>
-  <si>
-    <t>BalanceKp (float)</t>
-  </si>
-  <si>
-    <t>Request Drive Config</t>
-  </si>
-  <si>
-    <t>Response Drive Config</t>
-  </si>
-  <si>
-    <t>BalanceKd (float)</t>
-  </si>
-  <si>
-    <t>CRC32 (payload)</t>
-  </si>
-  <si>
-    <t>See Typelist</t>
-  </si>
-  <si>
-    <t>Command</t>
   </si>
   <si>
     <t>Page Data</t>
@@ -160,9 +51,6 @@
   </si>
   <si>
     <t>Response Flash Page</t>
-  </si>
-  <si>
-    <t>Set Flash Page</t>
   </si>
   <si>
     <t>0xAA</t>
@@ -227,23 +115,24 @@
   <si>
     <t>Result (enum)</t>
   </si>
+  <si>
+    <t>Request IMU Valueset</t>
+  </si>
+  <si>
+    <t>Set Index</t>
+  </si>
+  <si>
+    <t>Response IMU Valueset</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -272,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,19 +170,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -315,20 +192,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="18">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -413,15 +278,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -445,151 +301,40 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -597,44 +342,53 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -643,68 +397,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -712,6 +406,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -2556,237 +2251,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02CD1642-79E7-4DD6-9623-A45070CE8EAF}">
-  <dimension ref="A2:D17"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41:C42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2">
-        <f>SUM(D:D)</f>
-        <v>700</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>50</v>
-      </c>
-      <c r="D6">
-        <f>(1000/C6)*B6</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>50</v>
-      </c>
-      <c r="D7">
-        <f t="shared" ref="D7:D17" si="0">(1000/C7)*B7</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>50</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>50</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>50</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>50</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12">
-        <v>50</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>50</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>50</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>4</v>
-      </c>
-      <c r="C16">
-        <v>50</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>4</v>
-      </c>
-      <c r="C17">
-        <v>50</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A15:D15"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1AC88FD-8444-4667-A8F6-2D07972D95E5}">
   <dimension ref="A2:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2813,199 +2282,199 @@
       <c r="E2" s="1">
         <v>4</v>
       </c>
-      <c r="F2" s="33"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="35"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="26"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="40"/>
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="31"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="19" t="s">
-        <v>28</v>
+      <c r="B6" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="8" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="18">
+      <c r="B7" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" s="7">
         <v>1</v>
       </c>
-      <c r="E7" s="64" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
+      <c r="E7" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="22">
+      <c r="B8" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="11">
         <v>2</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="21"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="44" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="20">
+      <c r="B9" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="36"/>
+      <c r="D9" s="9">
         <v>3</v>
       </c>
-      <c r="E9" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="41"/>
+      <c r="E9" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="22">
+      <c r="B10" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="36"/>
+      <c r="D10" s="11">
         <v>4</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="21"/>
+      <c r="E10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="22">
+      <c r="B11" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="35"/>
+      <c r="D11" s="11">
         <v>5</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="22">
+      <c r="B12" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="11">
         <v>6</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>51</v>
+      <c r="E12" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="24">
+      <c r="B13" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="13">
         <v>7</v>
       </c>
-      <c r="E13" s="64" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="64"/>
+      <c r="E13" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="32"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="65" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="66"/>
-      <c r="D14" s="24">
+      <c r="B14" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="13">
         <v>8</v>
       </c>
-      <c r="E14" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
+      <c r="E14" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="18">
+      <c r="B15" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="23"/>
+      <c r="D15" s="7">
         <v>255</v>
       </c>
-      <c r="E15" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="E15" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
     </row>
     <row r="25" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E25" s="28"/>
+      <c r="E25" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -3033,42 +2502,42 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB83D9D3-B3A2-4544-B5AF-185922725977}">
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E29:E30"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="23"/>
-    <col min="4" max="4" width="10.42578125" style="26" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="12"/>
+    <col min="4" max="4" width="10.42578125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>52</v>
+      <c r="A1" s="12" t="s">
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>57</v>
+        <v>19</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="23">
+      <c r="A2" s="12">
         <v>3</v>
       </c>
       <c r="B2">
@@ -3078,7 +2547,7 @@
         <f t="shared" ref="C2:C28" si="0">13.8939*A2^-1.2423</f>
         <v>3.548921834194934</v>
       </c>
-      <c r="D2" s="27">
+      <c r="D2" s="16">
         <f>IF(C2/(B2/100)&gt;=100,(C2/(B2/100)-100)/100,(100-C2/(B2/100))/100)</f>
         <v>4.3800539469098114E-2</v>
       </c>
@@ -3090,7 +2559,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="23">
+      <c r="A3" s="12">
         <v>2.9</v>
       </c>
       <c r="B3">
@@ -3100,13 +2569,13 @@
         <f t="shared" si="0"/>
         <v>3.70157996594771</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="16">
         <f t="shared" ref="D3:D28" si="1">IF(C3/(B3/100)&gt;=100,(C3/(B3/100)-100)/100,(100-C3/(B3/100))/100)</f>
         <v>5.1585217598781125E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23">
+      <c r="A4" s="12">
         <v>2.8</v>
       </c>
       <c r="B4">
@@ -3116,13 +2585,13 @@
         <f t="shared" si="0"/>
         <v>3.8665154191003568</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="16">
         <f t="shared" si="1"/>
         <v>2.8328568909669515E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="23">
+      <c r="A5" s="12">
         <v>2.7</v>
       </c>
       <c r="B5">
@@ -3132,13 +2601,13 @@
         <f t="shared" si="0"/>
         <v>4.0452089974929528</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="16">
         <f t="shared" si="1"/>
         <v>3.1941070789018651E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="23">
+      <c r="A6" s="12">
         <v>2.6</v>
       </c>
       <c r="B6">
@@ -3148,13 +2617,13 @@
         <f t="shared" si="0"/>
         <v>4.2393842164859761</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="16">
         <f t="shared" si="1"/>
         <v>1.4523196085477252E-4</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="23">
+      <c r="A7" s="12">
         <v>2.5</v>
       </c>
       <c r="B7">
@@ -3164,13 +2633,13 @@
         <f t="shared" si="0"/>
         <v>4.4510584360155736</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="16">
         <f t="shared" si="1"/>
         <v>6.4601705322381523E-3</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="23">
+      <c r="A8" s="12">
         <v>2.4</v>
       </c>
       <c r="B8">
@@ -3180,13 +2649,13 @@
         <f t="shared" si="0"/>
         <v>4.682607357575721</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="16">
         <f t="shared" si="1"/>
         <v>1.6258958492495451E-2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="23">
+      <c r="A9" s="12">
         <v>2.2999999999999998</v>
       </c>
       <c r="B9">
@@ -3196,13 +2665,13 @@
         <f t="shared" si="0"/>
         <v>4.9368471143110719</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="16">
         <f t="shared" si="1"/>
         <v>2.0466842398596866E-2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="23">
+      <c r="A10" s="12">
         <v>2.2000000000000002</v>
       </c>
       <c r="B10">
@@ -3212,13 +2681,13 @@
         <f t="shared" si="0"/>
         <v>5.2171397761153218</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="16">
         <f t="shared" si="1"/>
         <v>2.6653026844156359E-2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="23">
+      <c r="A11" s="12">
         <v>2.1</v>
       </c>
       <c r="B11">
@@ -3228,13 +2697,13 @@
         <f t="shared" si="0"/>
         <v>5.5275303890992085</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="16">
         <f t="shared" si="1"/>
         <v>2.684324135577313E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="23">
+      <c r="A12" s="12">
         <v>2</v>
       </c>
       <c r="B12">
@@ -3244,13 +2713,13 @@
         <f t="shared" si="0"/>
         <v>5.8729270339689208</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="16">
         <f t="shared" si="1"/>
         <v>1.4609558058905918E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="23">
+      <c r="A13" s="12">
         <v>1.9</v>
       </c>
       <c r="B13">
@@ -3260,13 +2729,13 @@
         <f t="shared" si="0"/>
         <v>6.2593403997065415</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="16">
         <f t="shared" si="1"/>
         <v>2.8052732964822694E-2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="23">
+      <c r="A14" s="12">
         <v>1.8</v>
       </c>
       <c r="B14">
@@ -3276,13 +2745,13 @@
         <f t="shared" si="0"/>
         <v>6.6942069702755083</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="16">
         <f t="shared" si="1"/>
         <v>2.1314770427557334E-2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="23">
+      <c r="A15" s="12">
         <v>1.7</v>
       </c>
       <c r="B15">
@@ -3292,13 +2761,13 @@
         <f t="shared" si="0"/>
         <v>7.1868316832400545</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="16">
         <f t="shared" si="1"/>
         <v>1.2797845708783768E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="23">
+      <c r="A16" s="12">
         <v>1.6</v>
       </c>
       <c r="B16">
@@ -3308,13 +2777,13 @@
         <f t="shared" si="0"/>
         <v>7.7490045215398959</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="16">
         <f t="shared" si="1"/>
         <v>6.5378818538594889E-3</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="23">
+      <c r="A17" s="12">
         <v>1.5</v>
       </c>
       <c r="B17">
@@ -3324,13 +2793,13 @@
         <f t="shared" si="0"/>
         <v>8.3958756488752844</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="16">
         <f t="shared" si="1"/>
         <v>9.1196693359717074E-3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="23">
+      <c r="A18" s="12">
         <v>1.4</v>
       </c>
       <c r="B18">
@@ -3340,13 +2809,13 @@
         <f t="shared" si="0"/>
         <v>9.147223909086069</v>
       </c>
-      <c r="D18" s="27">
+      <c r="D18" s="16">
         <f t="shared" si="1"/>
         <v>2.089552556764147E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="23">
+      <c r="A19" s="12">
         <v>1.3</v>
       </c>
       <c r="B19">
@@ -3356,13 +2825,13 @@
         <f t="shared" si="0"/>
         <v>10.029339718465538</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="16">
         <f t="shared" si="1"/>
         <v>3.6088813891067988E-2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="23">
+      <c r="A20" s="12">
         <v>1.2</v>
       </c>
       <c r="B20">
@@ -3372,13 +2841,13 @@
         <f t="shared" si="0"/>
         <v>11.077896590425372</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D20" s="16">
         <f t="shared" si="1"/>
         <v>4.1155694588850621E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="23">
+      <c r="A21" s="12">
         <v>1.1000000000000001</v>
       </c>
       <c r="B21">
@@ -3388,13 +2857,13 @@
         <f t="shared" si="0"/>
         <v>12.3424687410738</v>
       </c>
-      <c r="D21" s="27">
+      <c r="D21" s="16">
         <f t="shared" si="1"/>
         <v>4.1733793394891305E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="23">
+      <c r="A22" s="12">
         <v>1</v>
       </c>
       <c r="B22">
@@ -3404,13 +2873,13 @@
         <f t="shared" si="0"/>
         <v>13.8939</v>
       </c>
-      <c r="D22" s="27">
+      <c r="D22" s="16">
         <f t="shared" si="1"/>
         <v>3.2458217270195037E-2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="23">
+      <c r="A23" s="12">
         <v>0.9</v>
       </c>
       <c r="B23">
@@ -3420,13 +2889,13 @@
         <f t="shared" si="0"/>
         <v>15.836846207410774</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D23" s="16">
         <f t="shared" si="1"/>
         <v>2.7220748930542129E-2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="23">
+      <c r="A24" s="12">
         <v>0.8</v>
       </c>
       <c r="B24">
@@ -3436,13 +2905,13 @@
         <f t="shared" si="0"/>
         <v>18.33223762173391</v>
       </c>
-      <c r="D24" s="27">
+      <c r="D24" s="16">
         <f t="shared" si="1"/>
         <v>2.9012837831890296E-2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="23">
+      <c r="A25" s="12">
         <v>0.7</v>
       </c>
       <c r="B25">
@@ -3452,13 +2921,13 @@
         <f t="shared" si="0"/>
         <v>21.640080582537596</v>
       </c>
-      <c r="D25" s="27">
+      <c r="D25" s="16">
         <f t="shared" si="1"/>
         <v>2.3462067575018182E-2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="23">
+      <c r="A26" s="12">
         <v>0.6</v>
       </c>
       <c r="B26">
@@ -3468,13 +2937,13 @@
         <f t="shared" si="0"/>
         <v>26.207576996524558</v>
       </c>
-      <c r="D26" s="27">
+      <c r="D26" s="16">
         <f t="shared" si="1"/>
         <v>1.8186925276971523E-3</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="23">
+      <c r="A27" s="12">
         <v>0.5</v>
       </c>
       <c r="B27">
@@ -3484,13 +2953,13 @@
         <f t="shared" si="0"/>
         <v>32.869548028343772</v>
       </c>
-      <c r="D27" s="27">
+      <c r="D27" s="16">
         <f t="shared" si="1"/>
         <v>4.5705387635626947E-3</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="23">
+      <c r="A28" s="12">
         <v>0.4</v>
       </c>
       <c r="B28">
@@ -3500,7 +2969,7 @@
         <f t="shared" si="0"/>
         <v>43.369562540006292</v>
       </c>
-      <c r="D28" s="27">
+      <c r="D28" s="16">
         <f t="shared" si="1"/>
         <v>7.6702148460930888E-2</v>
       </c>
@@ -3512,492 +2981,132 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD17DA2-D66C-4765-8B42-9B8593C77046}">
-  <dimension ref="B2:V23"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E30275A-3223-4A58-A1B9-300EAD4A76F7}">
+  <dimension ref="A2:M16"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="7.85546875" customWidth="1"/>
-    <col min="4" max="13" width="8" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="11.42578125" customWidth="1"/>
-    <col min="26" max="26" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
       <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="31"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" s="20">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E7" s="39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="19">
         <v>2</v>
       </c>
-      <c r="E2" s="1">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1">
-        <v>5</v>
-      </c>
-      <c r="H2" s="1">
-        <v>6</v>
-      </c>
-      <c r="I2" s="1">
-        <v>7</v>
-      </c>
-      <c r="J2" s="1">
-        <v>8</v>
-      </c>
-      <c r="K2" s="1">
-        <v>9</v>
-      </c>
-      <c r="L2" s="1">
-        <v>10</v>
-      </c>
-      <c r="M2" s="1">
-        <v>11</v>
-      </c>
-      <c r="N2" s="1">
-        <v>12</v>
-      </c>
-      <c r="O2" s="33"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="1">
-        <f>N2+64</f>
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="E8" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="62" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="40"/>
-    </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-    </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="32"/>
-      <c r="S5" s="32"/>
-      <c r="T5" s="32"/>
-      <c r="U5" s="32"/>
-      <c r="V5" s="32"/>
-    </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="32"/>
-      <c r="S6" s="32"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="32"/>
-      <c r="V6" s="32"/>
-    </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="32"/>
-      <c r="T7" s="32"/>
-      <c r="U7" s="32"/>
-      <c r="V7" s="32"/>
-    </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="32"/>
-      <c r="T8" s="32"/>
-      <c r="U8" s="32"/>
-      <c r="V8" s="32"/>
-    </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="32"/>
-      <c r="T9" s="32"/>
-      <c r="U9" s="32"/>
-      <c r="V9" s="32"/>
-    </row>
-    <row r="15" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F15" s="61" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="J15" s="12">
-        <v>8</v>
-      </c>
-      <c r="K15" s="12">
-        <v>9</v>
-      </c>
-      <c r="L15" s="12">
-        <v>10</v>
-      </c>
-      <c r="M15" s="12">
-        <v>11</v>
-      </c>
-      <c r="N15" s="12">
-        <v>12</v>
-      </c>
-      <c r="O15" s="12">
-        <v>13</v>
-      </c>
-      <c r="P15" s="12">
-        <v>14</v>
-      </c>
-      <c r="Q15" s="12">
-        <v>15</v>
-      </c>
-      <c r="R15" s="12">
-        <v>16</v>
-      </c>
-      <c r="S15" s="12">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F16" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="13">
-        <v>1</v>
-      </c>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-    </row>
-    <row r="17" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="F17" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="10">
-        <v>2</v>
-      </c>
-      <c r="J17" s="52" t="s">
-        <v>29</v>
-      </c>
-      <c r="K17" s="53"/>
-      <c r="L17" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="M17" s="60"/>
-      <c r="N17" s="60"/>
-      <c r="O17" s="60"/>
-      <c r="P17" s="60"/>
-      <c r="Q17" s="60"/>
-      <c r="R17" s="60"/>
-      <c r="S17" s="60"/>
-    </row>
-    <row r="18" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="F18" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="6">
-        <v>3</v>
-      </c>
-      <c r="J18" s="52" t="s">
-        <v>29</v>
-      </c>
-      <c r="K18" s="53"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
-    </row>
-    <row r="19" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="56" t="s">
-        <v>41</v>
-      </c>
-      <c r="G19" s="57"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="13">
-        <v>4</v>
-      </c>
-      <c r="J19" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="K19" s="50"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="50"/>
-      <c r="O19" s="50"/>
-      <c r="P19" s="50"/>
-      <c r="Q19" s="50"/>
-      <c r="R19" s="50"/>
-      <c r="S19" s="50"/>
-    </row>
-    <row r="20" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="F20" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="10">
-        <v>63</v>
-      </c>
-      <c r="J20" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="O20" s="47"/>
-      <c r="P20" s="47"/>
-      <c r="Q20" s="48"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="16"/>
-    </row>
-    <row r="21" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="F21" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="7">
-        <v>64</v>
-      </c>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
-      <c r="S21" s="16"/>
-    </row>
-    <row r="22" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="55" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="13">
-        <v>65</v>
-      </c>
-      <c r="J22" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="K22" s="50"/>
-      <c r="L22" s="50"/>
-      <c r="M22" s="51"/>
-      <c r="N22" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="O22" s="50"/>
-      <c r="P22" s="50"/>
-      <c r="Q22" s="51"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
-    </row>
-    <row r="23" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="O23" s="9"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E16" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="O2:U2"/>
-    <mergeCell ref="L17:S17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="N4:V4"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:V3"/>
-    <mergeCell ref="N5:V5"/>
-    <mergeCell ref="N6:V6"/>
-    <mergeCell ref="N7:V7"/>
-    <mergeCell ref="N8:V8"/>
-    <mergeCell ref="N9:V9"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="N20:Q20"/>
-    <mergeCell ref="N22:Q22"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:S19"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F19:H19"/>
+  <mergeCells count="7">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:M3"/>
+    <mergeCell ref="E4:M4"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>